<commit_message>
test disign at once
</commit_message>
<xml_diff>
--- a/Test Disign_1.xlsx
+++ b/Test Disign_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\GitReps\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D299459B-D48B-4BC9-BD71-A9F8EEF1FBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C1FB44-B0C6-4375-BABC-185D0AB82576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,10 +108,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -424,26 +424,26 @@
     </row>
     <row r="8" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
This is a checklist for design internet-store
</commit_message>
<xml_diff>
--- a/Test Disign_1.xlsx
+++ b/Test Disign_1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\GitReps\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1859CD39-0015-4888-92F1-ACD3E402DE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4959530E-AAF5-41B0-ACBF-8C04B0C5D35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rozetka checklist" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Equivalence partitioning</t>
   </si>
@@ -46,13 +47,97 @@
   </si>
   <si>
     <t>State transition Diagram</t>
+  </si>
+  <si>
+    <t>Главная страница</t>
+  </si>
+  <si>
+    <t>Сайт быстро загружается</t>
+  </si>
+  <si>
+    <t>Главное меню доступно и легко обнаруживается</t>
+  </si>
+  <si>
+    <t>Отображается логотип и брендинг</t>
+  </si>
+  <si>
+    <t>Баннеры и акции на главной странице привлекают внимание</t>
+  </si>
+  <si>
+    <t>Поиск находится на видном месте и легко доступен</t>
+  </si>
+  <si>
+    <t>Страница категории товаров</t>
+  </si>
+  <si>
+    <t>Страница быстро загружается</t>
+  </si>
+  <si>
+    <t>Главное меню отображает категорию товаров</t>
+  </si>
+  <si>
+    <t>Категории товаров ясно указаны в главном меню</t>
+  </si>
+  <si>
+    <t>Изображения товаров ясно отображают товар и его детали</t>
+  </si>
+  <si>
+    <t>Фильтры на странице позволяют уточнить результаты поиска</t>
+  </si>
+  <si>
+    <t>Страница товара</t>
+  </si>
+  <si>
+    <t>Страница товара быстро загружается</t>
+  </si>
+  <si>
+    <t>Отображается заголовок и цена товара</t>
+  </si>
+  <si>
+    <t>Изображения товара ясно отображают товар и его детали</t>
+  </si>
+  <si>
+    <t>Описание товара содержит достаточно информации</t>
+  </si>
+  <si>
+    <t>Кнопка "Купить" ясно отображается на странице товара</t>
+  </si>
+  <si>
+    <t>Страница корзины</t>
+  </si>
+  <si>
+    <t>Страница корзины быстро загружается</t>
+  </si>
+  <si>
+    <t>Все добавленные товары отображаются в корзине</t>
+  </si>
+  <si>
+    <t>Общая стоимость заказа и количество товаров ясно указаны</t>
+  </si>
+  <si>
+    <t>Кнопка "Оформить заказ" ясно отображается на странице корзины</t>
+  </si>
+  <si>
+    <t>Страница оформления заказа</t>
+  </si>
+  <si>
+    <t>Страница оформления заказа быстро загружается</t>
+  </si>
+  <si>
+    <t>Пользователь может легко вводить свои данные</t>
+  </si>
+  <si>
+    <t>Система оплаты безопасна и надежна</t>
+  </si>
+  <si>
+    <t>Политика доставки и возврата легко доступна и понятна</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,16 +152,28 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -99,11 +196,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -113,6 +225,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -449,4 +567,199 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8E9348-5C82-4941-B1A6-C3C460AFAB34}">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="47.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.85546875" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="47.85546875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>